<commit_message>
fix: update du modele excel
</commit_message>
<xml_diff>
--- a/packages/frontend/src/assets/files/modele.xlsx
+++ b/packages/frontend/src/assets/files/modele.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Google Drive/DomiFa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA9665A-8223-AD43-A822-CA2144F4D803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F9685-160D-8942-98E5-3984A0EFFD67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{78346249-D4CA-EC45-AC14-C98ADBF7EA96}"/>
   </bookViews>
   <sheets>
     <sheet name="DOMICILIES" sheetId="2" r:id="rId1"/>
-    <sheet name="LISTE DÉROULANTES" sheetId="3" r:id="rId2"/>
+    <sheet name="LISTE DÉROULANTES" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,9 +32,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
-  <si>
-    <t>testpapa@yopmail.com</t>
-  </si>
   <si>
     <t>PREMIERE</t>
   </si>
@@ -322,9 +319,6 @@
     <t>Marta</t>
   </si>
   <si>
-    <t>martadomifa@yopmail.com</t>
-  </si>
-  <si>
     <t>0142424241</t>
   </si>
   <si>
@@ -409,21 +403,6 @@
     <t>TÉLÉPHONE</t>
   </si>
   <si>
-    <r>
-      <t>TYPE DEMANDE</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
     <t>NOM
 AYANT-DROIT 1</t>
   </si>
@@ -471,9 +450,6 @@
 DU MÉNAGE</t>
   </si>
   <si>
-    <t>07/08/1978</t>
-  </si>
-  <si>
     <t>Sao Paulo, Brésil</t>
   </si>
   <si>
@@ -515,12 +491,36 @@
   <si>
     <t>12/09/2019</t>
   </si>
+  <si>
+    <t>domicilie1@yopmail.com</t>
+  </si>
+  <si>
+    <t>domicilie2@yopmail.com</t>
+  </si>
+  <si>
+    <r>
+      <t>TYPE DE DOMICILIATION</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>20/12/1991</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -654,13 +654,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="14"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
@@ -751,16 +744,16 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1563,7 +1556,7 @@
     <tableColumn id="7" xr3:uid="{622096D7-C4BC-B64C-919B-B72EE7A4C0BF}" name="EMAIL" dataDxfId="25" dataCellStyle="Lien hypertexte"/>
     <tableColumn id="8" xr3:uid="{F884A5C3-73BC-E342-8805-4EDAB8E82581}" name="TÉLÉPHONE" dataDxfId="24"/>
     <tableColumn id="13" xr3:uid="{3C10DDD9-6D43-A546-8B4B-5FBD905C8EB6}" name="STATUT DE LA _x000a_DOMICILIATION*" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{7CD8F7DE-C1DE-B845-8245-5CEDF419513E}" name="TYPE DEMANDE*" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{7CD8F7DE-C1DE-B845-8245-5CEDF419513E}" name="TYPE DE DOMICILIATION*" dataDxfId="22"/>
     <tableColumn id="9" xr3:uid="{124F3793-810B-D848-BD02-5E6E4E641891}" name="DATE DÉBUT_x000a_DOM ACTUELLE*" dataDxfId="21"/>
     <tableColumn id="10" xr3:uid="{0A059673-6E52-DE4E-960E-C05551C5E9E4}" name="DATE FIN DE DOMICILIATION*" dataDxfId="20"/>
     <tableColumn id="11" xr3:uid="{90AD863A-15F7-3041-9A55-D165BF61B6AC}" name="DATE _x000a_1ere DOM" dataDxfId="19"/>
@@ -1890,10 +1883,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667784FF-BEC0-7A46-B044-88051932373E}">
   <dimension ref="A1:AF267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1919,168 +1912,168 @@
   <sheetData>
     <row r="1" spans="1:32" s="13" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="P1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="R1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AC1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="15" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>94</v>
-      </c>
       <c r="M2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="W2" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X2" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y2" s="20"/>
       <c r="Z2" s="20"/>
@@ -2093,58 +2086,58 @@
     </row>
     <row r="3" spans="1:32" s="15" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="L3" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
       <c r="P3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
@@ -2161,44 +2154,44 @@
     </row>
     <row r="4" spans="1:32" s="15" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>71</v>
-      </c>
       <c r="E4" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="22"/>
+        <v>88</v>
+      </c>
+      <c r="G4" s="21"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" s="14"/>
       <c r="N4" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
@@ -2219,48 +2212,48 @@
     </row>
     <row r="5" spans="1:32" s="15" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="14" t="s">
-        <v>62</v>
-      </c>
       <c r="I5" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
@@ -2286,7 +2279,7 @@
       <c r="D6" s="20"/>
       <c r="E6" s="14"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="22"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -2316,11 +2309,11 @@
     <row r="7" spans="1:32" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="23"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="20"/>
       <c r="E7" s="14"/>
       <c r="F7" s="20"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -2354,7 +2347,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="14"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -2388,7 +2381,7 @@
       <c r="D9" s="20"/>
       <c r="E9" s="14"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -2422,7 +2415,7 @@
       <c r="D10" s="20"/>
       <c r="E10" s="14"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -2456,7 +2449,7 @@
       <c r="D11" s="20"/>
       <c r="E11" s="14"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -2490,7 +2483,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="14"/>
       <c r="F12" s="20"/>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -2524,7 +2517,7 @@
       <c r="D13" s="20"/>
       <c r="E13" s="14"/>
       <c r="F13" s="20"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -2558,7 +2551,7 @@
       <c r="D14" s="20"/>
       <c r="E14" s="14"/>
       <c r="F14" s="20"/>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -2592,7 +2585,7 @@
       <c r="D15" s="20"/>
       <c r="E15" s="14"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -2626,7 +2619,7 @@
       <c r="D16" s="20"/>
       <c r="E16" s="14"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -2660,7 +2653,7 @@
       <c r="D17" s="20"/>
       <c r="E17" s="14"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -2694,7 +2687,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="14"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -2728,7 +2721,7 @@
       <c r="D19" s="20"/>
       <c r="E19" s="14"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -2762,7 +2755,7 @@
       <c r="D20" s="20"/>
       <c r="E20" s="14"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -2796,7 +2789,7 @@
       <c r="D21" s="20"/>
       <c r="E21" s="14"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -2830,7 +2823,7 @@
       <c r="D22" s="20"/>
       <c r="E22" s="14"/>
       <c r="F22" s="20"/>
-      <c r="G22" s="24"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -2864,7 +2857,7 @@
       <c r="D23" s="20"/>
       <c r="E23" s="14"/>
       <c r="F23" s="20"/>
-      <c r="G23" s="24"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -2898,7 +2891,7 @@
       <c r="D24" s="20"/>
       <c r="E24" s="14"/>
       <c r="F24" s="20"/>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -2932,7 +2925,7 @@
       <c r="D25" s="20"/>
       <c r="E25" s="14"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -2966,7 +2959,7 @@
       <c r="D26" s="20"/>
       <c r="E26" s="14"/>
       <c r="F26" s="20"/>
-      <c r="G26" s="24"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -3000,7 +2993,7 @@
       <c r="D27" s="20"/>
       <c r="E27" s="14"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -3034,7 +3027,7 @@
       <c r="D28" s="20"/>
       <c r="E28" s="14"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="24"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -3068,7 +3061,7 @@
       <c r="D29" s="20"/>
       <c r="E29" s="14"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="24"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -3102,7 +3095,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="14"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="24"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -3136,7 +3129,7 @@
       <c r="D31" s="20"/>
       <c r="E31" s="14"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="24"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -3170,7 +3163,7 @@
       <c r="D32" s="20"/>
       <c r="E32" s="14"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -3204,7 +3197,7 @@
       <c r="D33" s="20"/>
       <c r="E33" s="14"/>
       <c r="F33" s="20"/>
-      <c r="G33" s="24"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -3238,7 +3231,7 @@
       <c r="D34" s="20"/>
       <c r="E34" s="14"/>
       <c r="F34" s="20"/>
-      <c r="G34" s="24"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -3272,7 +3265,7 @@
       <c r="D35" s="20"/>
       <c r="E35" s="14"/>
       <c r="F35" s="20"/>
-      <c r="G35" s="24"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -3306,7 +3299,7 @@
       <c r="D36" s="20"/>
       <c r="E36" s="14"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -3340,7 +3333,7 @@
       <c r="D37" s="20"/>
       <c r="E37" s="14"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="24"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -3374,7 +3367,7 @@
       <c r="D38" s="20"/>
       <c r="E38" s="14"/>
       <c r="F38" s="20"/>
-      <c r="G38" s="24"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -3408,7 +3401,7 @@
       <c r="D39" s="20"/>
       <c r="E39" s="14"/>
       <c r="F39" s="20"/>
-      <c r="G39" s="24"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -3442,7 +3435,7 @@
       <c r="D40" s="20"/>
       <c r="E40" s="14"/>
       <c r="F40" s="20"/>
-      <c r="G40" s="24"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -3476,7 +3469,7 @@
       <c r="D41" s="20"/>
       <c r="E41" s="14"/>
       <c r="F41" s="20"/>
-      <c r="G41" s="24"/>
+      <c r="G41" s="23"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -3510,7 +3503,7 @@
       <c r="D42" s="20"/>
       <c r="E42" s="14"/>
       <c r="F42" s="20"/>
-      <c r="G42" s="24"/>
+      <c r="G42" s="23"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -3544,7 +3537,7 @@
       <c r="D43" s="20"/>
       <c r="E43" s="14"/>
       <c r="F43" s="20"/>
-      <c r="G43" s="24"/>
+      <c r="G43" s="23"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -3578,7 +3571,7 @@
       <c r="D44" s="20"/>
       <c r="E44" s="14"/>
       <c r="F44" s="20"/>
-      <c r="G44" s="24"/>
+      <c r="G44" s="23"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -3612,7 +3605,7 @@
       <c r="D45" s="20"/>
       <c r="E45" s="14"/>
       <c r="F45" s="20"/>
-      <c r="G45" s="24"/>
+      <c r="G45" s="23"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -3646,7 +3639,7 @@
       <c r="D46" s="20"/>
       <c r="E46" s="14"/>
       <c r="F46" s="20"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -3680,7 +3673,7 @@
       <c r="D47" s="20"/>
       <c r="E47" s="14"/>
       <c r="F47" s="20"/>
-      <c r="G47" s="24"/>
+      <c r="G47" s="23"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -3714,7 +3707,7 @@
       <c r="D48" s="20"/>
       <c r="E48" s="14"/>
       <c r="F48" s="20"/>
-      <c r="G48" s="24"/>
+      <c r="G48" s="23"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
@@ -3748,7 +3741,7 @@
       <c r="D49" s="20"/>
       <c r="E49" s="14"/>
       <c r="F49" s="20"/>
-      <c r="G49" s="24"/>
+      <c r="G49" s="23"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
@@ -3782,7 +3775,7 @@
       <c r="D50" s="20"/>
       <c r="E50" s="14"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="24"/>
+      <c r="G50" s="23"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
@@ -3816,7 +3809,7 @@
       <c r="D51" s="20"/>
       <c r="E51" s="14"/>
       <c r="F51" s="20"/>
-      <c r="G51" s="24"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
@@ -3850,7 +3843,7 @@
       <c r="D52" s="20"/>
       <c r="E52" s="14"/>
       <c r="F52" s="20"/>
-      <c r="G52" s="24"/>
+      <c r="G52" s="23"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
@@ -3884,7 +3877,7 @@
       <c r="D53" s="20"/>
       <c r="E53" s="14"/>
       <c r="F53" s="20"/>
-      <c r="G53" s="24"/>
+      <c r="G53" s="23"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
@@ -3918,7 +3911,7 @@
       <c r="D54" s="20"/>
       <c r="E54" s="14"/>
       <c r="F54" s="20"/>
-      <c r="G54" s="24"/>
+      <c r="G54" s="23"/>
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -3952,7 +3945,7 @@
       <c r="D55" s="20"/>
       <c r="E55" s="14"/>
       <c r="F55" s="20"/>
-      <c r="G55" s="24"/>
+      <c r="G55" s="23"/>
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
@@ -3986,7 +3979,7 @@
       <c r="D56" s="20"/>
       <c r="E56" s="14"/>
       <c r="F56" s="20"/>
-      <c r="G56" s="24"/>
+      <c r="G56" s="23"/>
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
@@ -4020,7 +4013,7 @@
       <c r="D57" s="20"/>
       <c r="E57" s="14"/>
       <c r="F57" s="20"/>
-      <c r="G57" s="24"/>
+      <c r="G57" s="23"/>
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
@@ -4054,7 +4047,7 @@
       <c r="D58" s="20"/>
       <c r="E58" s="14"/>
       <c r="F58" s="20"/>
-      <c r="G58" s="24"/>
+      <c r="G58" s="23"/>
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -4088,7 +4081,7 @@
       <c r="D59" s="20"/>
       <c r="E59" s="14"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="24"/>
+      <c r="G59" s="23"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
@@ -4122,7 +4115,7 @@
       <c r="D60" s="20"/>
       <c r="E60" s="14"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="24"/>
+      <c r="G60" s="23"/>
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
@@ -4156,7 +4149,7 @@
       <c r="D61" s="20"/>
       <c r="E61" s="14"/>
       <c r="F61" s="20"/>
-      <c r="G61" s="24"/>
+      <c r="G61" s="23"/>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
@@ -4190,7 +4183,7 @@
       <c r="D62" s="20"/>
       <c r="E62" s="14"/>
       <c r="F62" s="20"/>
-      <c r="G62" s="24"/>
+      <c r="G62" s="23"/>
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
@@ -4224,7 +4217,7 @@
       <c r="D63" s="20"/>
       <c r="E63" s="14"/>
       <c r="F63" s="20"/>
-      <c r="G63" s="24"/>
+      <c r="G63" s="23"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
@@ -4258,7 +4251,7 @@
       <c r="D64" s="20"/>
       <c r="E64" s="14"/>
       <c r="F64" s="20"/>
-      <c r="G64" s="24"/>
+      <c r="G64" s="23"/>
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
@@ -4292,7 +4285,7 @@
       <c r="D65" s="20"/>
       <c r="E65" s="14"/>
       <c r="F65" s="20"/>
-      <c r="G65" s="24"/>
+      <c r="G65" s="23"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
@@ -4326,7 +4319,7 @@
       <c r="D66" s="20"/>
       <c r="E66" s="14"/>
       <c r="F66" s="20"/>
-      <c r="G66" s="24"/>
+      <c r="G66" s="23"/>
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
@@ -4360,7 +4353,7 @@
       <c r="D67" s="20"/>
       <c r="E67" s="14"/>
       <c r="F67" s="20"/>
-      <c r="G67" s="24"/>
+      <c r="G67" s="23"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
@@ -4394,7 +4387,7 @@
       <c r="D68" s="20"/>
       <c r="E68" s="14"/>
       <c r="F68" s="20"/>
-      <c r="G68" s="24"/>
+      <c r="G68" s="23"/>
       <c r="H68" s="14"/>
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
@@ -4428,7 +4421,7 @@
       <c r="D69" s="20"/>
       <c r="E69" s="14"/>
       <c r="F69" s="20"/>
-      <c r="G69" s="24"/>
+      <c r="G69" s="23"/>
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
@@ -4462,7 +4455,7 @@
       <c r="D70" s="20"/>
       <c r="E70" s="14"/>
       <c r="F70" s="20"/>
-      <c r="G70" s="24"/>
+      <c r="G70" s="23"/>
       <c r="H70" s="14"/>
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
@@ -4496,7 +4489,7 @@
       <c r="D71" s="20"/>
       <c r="E71" s="14"/>
       <c r="F71" s="20"/>
-      <c r="G71" s="24"/>
+      <c r="G71" s="23"/>
       <c r="H71" s="14"/>
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
@@ -4530,7 +4523,7 @@
       <c r="D72" s="20"/>
       <c r="E72" s="14"/>
       <c r="F72" s="20"/>
-      <c r="G72" s="24"/>
+      <c r="G72" s="23"/>
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
@@ -4564,7 +4557,7 @@
       <c r="D73" s="20"/>
       <c r="E73" s="14"/>
       <c r="F73" s="20"/>
-      <c r="G73" s="24"/>
+      <c r="G73" s="23"/>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
@@ -4598,7 +4591,7 @@
       <c r="D74" s="20"/>
       <c r="E74" s="14"/>
       <c r="F74" s="20"/>
-      <c r="G74" s="24"/>
+      <c r="G74" s="23"/>
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
@@ -4632,7 +4625,7 @@
       <c r="D75" s="20"/>
       <c r="E75" s="14"/>
       <c r="F75" s="20"/>
-      <c r="G75" s="24"/>
+      <c r="G75" s="23"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
@@ -4666,7 +4659,7 @@
       <c r="D76" s="20"/>
       <c r="E76" s="14"/>
       <c r="F76" s="20"/>
-      <c r="G76" s="24"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
@@ -4700,7 +4693,7 @@
       <c r="D77" s="20"/>
       <c r="E77" s="14"/>
       <c r="F77" s="20"/>
-      <c r="G77" s="24"/>
+      <c r="G77" s="23"/>
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
@@ -4734,7 +4727,7 @@
       <c r="D78" s="20"/>
       <c r="E78" s="14"/>
       <c r="F78" s="20"/>
-      <c r="G78" s="24"/>
+      <c r="G78" s="23"/>
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
@@ -4768,7 +4761,7 @@
       <c r="D79" s="20"/>
       <c r="E79" s="14"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="24"/>
+      <c r="G79" s="23"/>
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
@@ -4802,7 +4795,7 @@
       <c r="D80" s="20"/>
       <c r="E80" s="14"/>
       <c r="F80" s="20"/>
-      <c r="G80" s="24"/>
+      <c r="G80" s="23"/>
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
@@ -4836,7 +4829,7 @@
       <c r="D81" s="20"/>
       <c r="E81" s="14"/>
       <c r="F81" s="20"/>
-      <c r="G81" s="24"/>
+      <c r="G81" s="23"/>
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
@@ -4870,7 +4863,7 @@
       <c r="D82" s="20"/>
       <c r="E82" s="14"/>
       <c r="F82" s="20"/>
-      <c r="G82" s="24"/>
+      <c r="G82" s="23"/>
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
@@ -4904,7 +4897,7 @@
       <c r="D83" s="20"/>
       <c r="E83" s="14"/>
       <c r="F83" s="20"/>
-      <c r="G83" s="24"/>
+      <c r="G83" s="23"/>
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
@@ -4938,7 +4931,7 @@
       <c r="D84" s="20"/>
       <c r="E84" s="14"/>
       <c r="F84" s="20"/>
-      <c r="G84" s="24"/>
+      <c r="G84" s="23"/>
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
@@ -4972,7 +4965,7 @@
       <c r="D85" s="20"/>
       <c r="E85" s="14"/>
       <c r="F85" s="20"/>
-      <c r="G85" s="24"/>
+      <c r="G85" s="23"/>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
@@ -5006,7 +4999,7 @@
       <c r="D86" s="20"/>
       <c r="E86" s="14"/>
       <c r="F86" s="20"/>
-      <c r="G86" s="24"/>
+      <c r="G86" s="23"/>
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
@@ -5040,7 +5033,7 @@
       <c r="D87" s="20"/>
       <c r="E87" s="14"/>
       <c r="F87" s="20"/>
-      <c r="G87" s="24"/>
+      <c r="G87" s="23"/>
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
@@ -5074,7 +5067,7 @@
       <c r="D88" s="20"/>
       <c r="E88" s="14"/>
       <c r="F88" s="20"/>
-      <c r="G88" s="24"/>
+      <c r="G88" s="23"/>
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
@@ -5108,7 +5101,7 @@
       <c r="D89" s="20"/>
       <c r="E89" s="14"/>
       <c r="F89" s="20"/>
-      <c r="G89" s="24"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
@@ -5142,7 +5135,7 @@
       <c r="D90" s="20"/>
       <c r="E90" s="14"/>
       <c r="F90" s="20"/>
-      <c r="G90" s="24"/>
+      <c r="G90" s="23"/>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
@@ -5176,7 +5169,7 @@
       <c r="D91" s="20"/>
       <c r="E91" s="14"/>
       <c r="F91" s="20"/>
-      <c r="G91" s="24"/>
+      <c r="G91" s="23"/>
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
@@ -5210,7 +5203,7 @@
       <c r="D92" s="20"/>
       <c r="E92" s="14"/>
       <c r="F92" s="20"/>
-      <c r="G92" s="24"/>
+      <c r="G92" s="23"/>
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
@@ -5244,7 +5237,7 @@
       <c r="D93" s="20"/>
       <c r="E93" s="14"/>
       <c r="F93" s="20"/>
-      <c r="G93" s="24"/>
+      <c r="G93" s="23"/>
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
@@ -5278,7 +5271,7 @@
       <c r="D94" s="20"/>
       <c r="E94" s="14"/>
       <c r="F94" s="20"/>
-      <c r="G94" s="24"/>
+      <c r="G94" s="23"/>
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
@@ -5312,7 +5305,7 @@
       <c r="D95" s="20"/>
       <c r="E95" s="14"/>
       <c r="F95" s="20"/>
-      <c r="G95" s="24"/>
+      <c r="G95" s="23"/>
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
@@ -5346,7 +5339,7 @@
       <c r="D96" s="20"/>
       <c r="E96" s="14"/>
       <c r="F96" s="20"/>
-      <c r="G96" s="24"/>
+      <c r="G96" s="23"/>
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
       <c r="J96" s="14"/>
@@ -5380,7 +5373,7 @@
       <c r="D97" s="20"/>
       <c r="E97" s="14"/>
       <c r="F97" s="20"/>
-      <c r="G97" s="24"/>
+      <c r="G97" s="23"/>
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
@@ -5414,7 +5407,7 @@
       <c r="D98" s="20"/>
       <c r="E98" s="14"/>
       <c r="F98" s="20"/>
-      <c r="G98" s="24"/>
+      <c r="G98" s="23"/>
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="14"/>
@@ -5448,7 +5441,7 @@
       <c r="D99" s="20"/>
       <c r="E99" s="14"/>
       <c r="F99" s="20"/>
-      <c r="G99" s="24"/>
+      <c r="G99" s="23"/>
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
@@ -5482,7 +5475,7 @@
       <c r="D100" s="20"/>
       <c r="E100" s="14"/>
       <c r="F100" s="20"/>
-      <c r="G100" s="24"/>
+      <c r="G100" s="23"/>
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
       <c r="J100" s="14"/>
@@ -5516,7 +5509,7 @@
       <c r="D101" s="20"/>
       <c r="E101" s="14"/>
       <c r="F101" s="20"/>
-      <c r="G101" s="24"/>
+      <c r="G101" s="23"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
@@ -5550,7 +5543,7 @@
       <c r="D102" s="20"/>
       <c r="E102" s="14"/>
       <c r="F102" s="20"/>
-      <c r="G102" s="24"/>
+      <c r="G102" s="23"/>
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
@@ -5584,7 +5577,7 @@
       <c r="D103" s="20"/>
       <c r="E103" s="14"/>
       <c r="F103" s="20"/>
-      <c r="G103" s="24"/>
+      <c r="G103" s="23"/>
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
@@ -5618,7 +5611,7 @@
       <c r="D104" s="20"/>
       <c r="E104" s="14"/>
       <c r="F104" s="20"/>
-      <c r="G104" s="24"/>
+      <c r="G104" s="23"/>
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
@@ -5652,7 +5645,7 @@
       <c r="D105" s="20"/>
       <c r="E105" s="14"/>
       <c r="F105" s="20"/>
-      <c r="G105" s="24"/>
+      <c r="G105" s="23"/>
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
@@ -5686,7 +5679,7 @@
       <c r="D106" s="20"/>
       <c r="E106" s="14"/>
       <c r="F106" s="20"/>
-      <c r="G106" s="24"/>
+      <c r="G106" s="23"/>
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
@@ -5720,7 +5713,7 @@
       <c r="D107" s="20"/>
       <c r="E107" s="14"/>
       <c r="F107" s="20"/>
-      <c r="G107" s="24"/>
+      <c r="G107" s="23"/>
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
@@ -5754,7 +5747,7 @@
       <c r="D108" s="20"/>
       <c r="E108" s="14"/>
       <c r="F108" s="20"/>
-      <c r="G108" s="24"/>
+      <c r="G108" s="23"/>
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="14"/>
@@ -5788,7 +5781,7 @@
       <c r="D109" s="20"/>
       <c r="E109" s="14"/>
       <c r="F109" s="20"/>
-      <c r="G109" s="24"/>
+      <c r="G109" s="23"/>
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="14"/>
@@ -5822,7 +5815,7 @@
       <c r="D110" s="20"/>
       <c r="E110" s="14"/>
       <c r="F110" s="20"/>
-      <c r="G110" s="24"/>
+      <c r="G110" s="23"/>
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="14"/>
@@ -5856,7 +5849,7 @@
       <c r="D111" s="20"/>
       <c r="E111" s="14"/>
       <c r="F111" s="20"/>
-      <c r="G111" s="24"/>
+      <c r="G111" s="23"/>
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="14"/>
@@ -5890,7 +5883,7 @@
       <c r="D112" s="20"/>
       <c r="E112" s="14"/>
       <c r="F112" s="20"/>
-      <c r="G112" s="24"/>
+      <c r="G112" s="23"/>
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
@@ -5924,7 +5917,7 @@
       <c r="D113" s="20"/>
       <c r="E113" s="14"/>
       <c r="F113" s="20"/>
-      <c r="G113" s="24"/>
+      <c r="G113" s="23"/>
       <c r="H113" s="14"/>
       <c r="I113" s="14"/>
       <c r="J113" s="14"/>
@@ -5958,7 +5951,7 @@
       <c r="D114" s="20"/>
       <c r="E114" s="14"/>
       <c r="F114" s="20"/>
-      <c r="G114" s="24"/>
+      <c r="G114" s="23"/>
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
@@ -5992,7 +5985,7 @@
       <c r="D115" s="20"/>
       <c r="E115" s="14"/>
       <c r="F115" s="20"/>
-      <c r="G115" s="24"/>
+      <c r="G115" s="23"/>
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
@@ -6026,7 +6019,7 @@
       <c r="D116" s="20"/>
       <c r="E116" s="14"/>
       <c r="F116" s="20"/>
-      <c r="G116" s="24"/>
+      <c r="G116" s="23"/>
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="14"/>
@@ -6060,7 +6053,7 @@
       <c r="D117" s="20"/>
       <c r="E117" s="14"/>
       <c r="F117" s="20"/>
-      <c r="G117" s="24"/>
+      <c r="G117" s="23"/>
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
       <c r="J117" s="14"/>
@@ -6094,7 +6087,7 @@
       <c r="D118" s="20"/>
       <c r="E118" s="14"/>
       <c r="F118" s="20"/>
-      <c r="G118" s="24"/>
+      <c r="G118" s="23"/>
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
       <c r="J118" s="14"/>
@@ -6128,7 +6121,7 @@
       <c r="D119" s="20"/>
       <c r="E119" s="14"/>
       <c r="F119" s="20"/>
-      <c r="G119" s="24"/>
+      <c r="G119" s="23"/>
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
       <c r="J119" s="14"/>
@@ -6162,7 +6155,7 @@
       <c r="D120" s="20"/>
       <c r="E120" s="14"/>
       <c r="F120" s="20"/>
-      <c r="G120" s="24"/>
+      <c r="G120" s="23"/>
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
       <c r="J120" s="14"/>
@@ -6196,7 +6189,7 @@
       <c r="D121" s="20"/>
       <c r="E121" s="14"/>
       <c r="F121" s="20"/>
-      <c r="G121" s="24"/>
+      <c r="G121" s="23"/>
       <c r="H121" s="14"/>
       <c r="I121" s="14"/>
       <c r="J121" s="14"/>
@@ -6230,7 +6223,7 @@
       <c r="D122" s="20"/>
       <c r="E122" s="14"/>
       <c r="F122" s="20"/>
-      <c r="G122" s="24"/>
+      <c r="G122" s="23"/>
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
       <c r="J122" s="14"/>
@@ -6264,7 +6257,7 @@
       <c r="D123" s="20"/>
       <c r="E123" s="14"/>
       <c r="F123" s="20"/>
-      <c r="G123" s="24"/>
+      <c r="G123" s="23"/>
       <c r="H123" s="14"/>
       <c r="I123" s="14"/>
       <c r="J123" s="14"/>
@@ -6298,7 +6291,7 @@
       <c r="D124" s="20"/>
       <c r="E124" s="14"/>
       <c r="F124" s="20"/>
-      <c r="G124" s="24"/>
+      <c r="G124" s="23"/>
       <c r="H124" s="14"/>
       <c r="I124" s="14"/>
       <c r="J124" s="14"/>
@@ -6332,7 +6325,7 @@
       <c r="D125" s="20"/>
       <c r="E125" s="14"/>
       <c r="F125" s="20"/>
-      <c r="G125" s="24"/>
+      <c r="G125" s="23"/>
       <c r="H125" s="14"/>
       <c r="I125" s="14"/>
       <c r="J125" s="14"/>
@@ -6366,7 +6359,7 @@
       <c r="D126" s="20"/>
       <c r="E126" s="14"/>
       <c r="F126" s="20"/>
-      <c r="G126" s="24"/>
+      <c r="G126" s="23"/>
       <c r="H126" s="14"/>
       <c r="I126" s="14"/>
       <c r="J126" s="14"/>
@@ -6400,7 +6393,7 @@
       <c r="D127" s="20"/>
       <c r="E127" s="14"/>
       <c r="F127" s="20"/>
-      <c r="G127" s="24"/>
+      <c r="G127" s="23"/>
       <c r="H127" s="14"/>
       <c r="I127" s="14"/>
       <c r="J127" s="14"/>
@@ -6434,7 +6427,7 @@
       <c r="D128" s="20"/>
       <c r="E128" s="14"/>
       <c r="F128" s="20"/>
-      <c r="G128" s="24"/>
+      <c r="G128" s="23"/>
       <c r="H128" s="14"/>
       <c r="I128" s="14"/>
       <c r="J128" s="14"/>
@@ -6468,7 +6461,7 @@
       <c r="D129" s="20"/>
       <c r="E129" s="14"/>
       <c r="F129" s="20"/>
-      <c r="G129" s="24"/>
+      <c r="G129" s="23"/>
       <c r="H129" s="14"/>
       <c r="I129" s="14"/>
       <c r="J129" s="14"/>
@@ -6502,7 +6495,7 @@
       <c r="D130" s="20"/>
       <c r="E130" s="14"/>
       <c r="F130" s="20"/>
-      <c r="G130" s="24"/>
+      <c r="G130" s="23"/>
       <c r="H130" s="14"/>
       <c r="I130" s="14"/>
       <c r="J130" s="14"/>
@@ -6536,7 +6529,7 @@
       <c r="D131" s="20"/>
       <c r="E131" s="14"/>
       <c r="F131" s="20"/>
-      <c r="G131" s="24"/>
+      <c r="G131" s="23"/>
       <c r="H131" s="14"/>
       <c r="I131" s="14"/>
       <c r="J131" s="14"/>
@@ -6570,7 +6563,7 @@
       <c r="D132" s="20"/>
       <c r="E132" s="14"/>
       <c r="F132" s="20"/>
-      <c r="G132" s="24"/>
+      <c r="G132" s="23"/>
       <c r="H132" s="14"/>
       <c r="I132" s="14"/>
       <c r="J132" s="14"/>
@@ -6604,7 +6597,7 @@
       <c r="D133" s="20"/>
       <c r="E133" s="14"/>
       <c r="F133" s="20"/>
-      <c r="G133" s="24"/>
+      <c r="G133" s="23"/>
       <c r="H133" s="14"/>
       <c r="I133" s="14"/>
       <c r="J133" s="14"/>
@@ -6638,7 +6631,7 @@
       <c r="D134" s="20"/>
       <c r="E134" s="14"/>
       <c r="F134" s="20"/>
-      <c r="G134" s="24"/>
+      <c r="G134" s="23"/>
       <c r="H134" s="14"/>
       <c r="I134" s="14"/>
       <c r="J134" s="14"/>
@@ -6672,7 +6665,7 @@
       <c r="D135" s="20"/>
       <c r="E135" s="14"/>
       <c r="F135" s="20"/>
-      <c r="G135" s="24"/>
+      <c r="G135" s="23"/>
       <c r="H135" s="14"/>
       <c r="I135" s="14"/>
       <c r="J135" s="14"/>
@@ -6706,7 +6699,7 @@
       <c r="D136" s="20"/>
       <c r="E136" s="14"/>
       <c r="F136" s="20"/>
-      <c r="G136" s="24"/>
+      <c r="G136" s="23"/>
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
       <c r="J136" s="14"/>
@@ -6740,7 +6733,7 @@
       <c r="D137" s="20"/>
       <c r="E137" s="14"/>
       <c r="F137" s="20"/>
-      <c r="G137" s="24"/>
+      <c r="G137" s="23"/>
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
       <c r="J137" s="14"/>
@@ -6774,7 +6767,7 @@
       <c r="D138" s="20"/>
       <c r="E138" s="14"/>
       <c r="F138" s="20"/>
-      <c r="G138" s="24"/>
+      <c r="G138" s="23"/>
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
       <c r="J138" s="14"/>
@@ -6808,7 +6801,7 @@
       <c r="D139" s="20"/>
       <c r="E139" s="14"/>
       <c r="F139" s="20"/>
-      <c r="G139" s="24"/>
+      <c r="G139" s="23"/>
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
       <c r="J139" s="14"/>
@@ -6842,7 +6835,7 @@
       <c r="D140" s="20"/>
       <c r="E140" s="14"/>
       <c r="F140" s="20"/>
-      <c r="G140" s="24"/>
+      <c r="G140" s="23"/>
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
       <c r="J140" s="14"/>
@@ -6876,7 +6869,7 @@
       <c r="D141" s="20"/>
       <c r="E141" s="14"/>
       <c r="F141" s="20"/>
-      <c r="G141" s="24"/>
+      <c r="G141" s="23"/>
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
       <c r="J141" s="14"/>
@@ -6910,7 +6903,7 @@
       <c r="D142" s="20"/>
       <c r="E142" s="14"/>
       <c r="F142" s="20"/>
-      <c r="G142" s="24"/>
+      <c r="G142" s="23"/>
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
       <c r="J142" s="14"/>
@@ -6944,7 +6937,7 @@
       <c r="D143" s="20"/>
       <c r="E143" s="14"/>
       <c r="F143" s="20"/>
-      <c r="G143" s="24"/>
+      <c r="G143" s="23"/>
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
       <c r="J143" s="14"/>
@@ -6978,7 +6971,7 @@
       <c r="D144" s="20"/>
       <c r="E144" s="14"/>
       <c r="F144" s="20"/>
-      <c r="G144" s="24"/>
+      <c r="G144" s="23"/>
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
       <c r="J144" s="14"/>
@@ -7012,7 +7005,7 @@
       <c r="D145" s="20"/>
       <c r="E145" s="14"/>
       <c r="F145" s="20"/>
-      <c r="G145" s="24"/>
+      <c r="G145" s="23"/>
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
       <c r="J145" s="14"/>
@@ -7046,7 +7039,7 @@
       <c r="D146" s="20"/>
       <c r="E146" s="14"/>
       <c r="F146" s="20"/>
-      <c r="G146" s="24"/>
+      <c r="G146" s="23"/>
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
       <c r="J146" s="14"/>
@@ -7080,7 +7073,7 @@
       <c r="D147" s="20"/>
       <c r="E147" s="14"/>
       <c r="F147" s="20"/>
-      <c r="G147" s="24"/>
+      <c r="G147" s="23"/>
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="14"/>
@@ -7114,7 +7107,7 @@
       <c r="D148" s="20"/>
       <c r="E148" s="14"/>
       <c r="F148" s="20"/>
-      <c r="G148" s="24"/>
+      <c r="G148" s="23"/>
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
       <c r="J148" s="14"/>
@@ -7148,7 +7141,7 @@
       <c r="D149" s="20"/>
       <c r="E149" s="14"/>
       <c r="F149" s="20"/>
-      <c r="G149" s="24"/>
+      <c r="G149" s="23"/>
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
       <c r="J149" s="14"/>
@@ -7182,7 +7175,7 @@
       <c r="D150" s="20"/>
       <c r="E150" s="14"/>
       <c r="F150" s="20"/>
-      <c r="G150" s="24"/>
+      <c r="G150" s="23"/>
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
       <c r="J150" s="14"/>
@@ -7216,7 +7209,7 @@
       <c r="D151" s="20"/>
       <c r="E151" s="14"/>
       <c r="F151" s="20"/>
-      <c r="G151" s="24"/>
+      <c r="G151" s="23"/>
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
       <c r="J151" s="14"/>
@@ -7250,7 +7243,7 @@
       <c r="D152" s="20"/>
       <c r="E152" s="14"/>
       <c r="F152" s="20"/>
-      <c r="G152" s="24"/>
+      <c r="G152" s="23"/>
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
       <c r="J152" s="14"/>
@@ -7284,7 +7277,7 @@
       <c r="D153" s="20"/>
       <c r="E153" s="14"/>
       <c r="F153" s="20"/>
-      <c r="G153" s="24"/>
+      <c r="G153" s="23"/>
       <c r="H153" s="14"/>
       <c r="I153" s="14"/>
       <c r="J153" s="14"/>
@@ -7318,7 +7311,7 @@
       <c r="D154" s="20"/>
       <c r="E154" s="14"/>
       <c r="F154" s="20"/>
-      <c r="G154" s="24"/>
+      <c r="G154" s="23"/>
       <c r="H154" s="14"/>
       <c r="I154" s="14"/>
       <c r="J154" s="14"/>
@@ -7352,7 +7345,7 @@
       <c r="D155" s="20"/>
       <c r="E155" s="14"/>
       <c r="F155" s="20"/>
-      <c r="G155" s="24"/>
+      <c r="G155" s="23"/>
       <c r="H155" s="14"/>
       <c r="I155" s="14"/>
       <c r="J155" s="14"/>
@@ -7386,7 +7379,7 @@
       <c r="D156" s="20"/>
       <c r="E156" s="14"/>
       <c r="F156" s="20"/>
-      <c r="G156" s="24"/>
+      <c r="G156" s="23"/>
       <c r="H156" s="14"/>
       <c r="I156" s="14"/>
       <c r="J156" s="14"/>
@@ -7420,7 +7413,7 @@
       <c r="D157" s="20"/>
       <c r="E157" s="14"/>
       <c r="F157" s="20"/>
-      <c r="G157" s="24"/>
+      <c r="G157" s="23"/>
       <c r="H157" s="14"/>
       <c r="I157" s="14"/>
       <c r="J157" s="14"/>
@@ -7454,7 +7447,7 @@
       <c r="D158" s="20"/>
       <c r="E158" s="14"/>
       <c r="F158" s="20"/>
-      <c r="G158" s="24"/>
+      <c r="G158" s="23"/>
       <c r="H158" s="14"/>
       <c r="I158" s="14"/>
       <c r="J158" s="14"/>
@@ -7488,7 +7481,7 @@
       <c r="D159" s="20"/>
       <c r="E159" s="14"/>
       <c r="F159" s="20"/>
-      <c r="G159" s="24"/>
+      <c r="G159" s="23"/>
       <c r="H159" s="14"/>
       <c r="I159" s="14"/>
       <c r="J159" s="14"/>
@@ -7522,7 +7515,7 @@
       <c r="D160" s="20"/>
       <c r="E160" s="14"/>
       <c r="F160" s="20"/>
-      <c r="G160" s="24"/>
+      <c r="G160" s="23"/>
       <c r="H160" s="14"/>
       <c r="I160" s="14"/>
       <c r="J160" s="14"/>
@@ -7556,7 +7549,7 @@
       <c r="D161" s="20"/>
       <c r="E161" s="14"/>
       <c r="F161" s="20"/>
-      <c r="G161" s="24"/>
+      <c r="G161" s="23"/>
       <c r="H161" s="14"/>
       <c r="I161" s="14"/>
       <c r="J161" s="14"/>
@@ -7590,7 +7583,7 @@
       <c r="D162" s="20"/>
       <c r="E162" s="14"/>
       <c r="F162" s="20"/>
-      <c r="G162" s="24"/>
+      <c r="G162" s="23"/>
       <c r="H162" s="14"/>
       <c r="I162" s="14"/>
       <c r="J162" s="14"/>
@@ -7624,7 +7617,7 @@
       <c r="D163" s="20"/>
       <c r="E163" s="14"/>
       <c r="F163" s="20"/>
-      <c r="G163" s="24"/>
+      <c r="G163" s="23"/>
       <c r="H163" s="14"/>
       <c r="I163" s="14"/>
       <c r="J163" s="14"/>
@@ -7658,7 +7651,7 @@
       <c r="D164" s="20"/>
       <c r="E164" s="14"/>
       <c r="F164" s="20"/>
-      <c r="G164" s="24"/>
+      <c r="G164" s="23"/>
       <c r="H164" s="14"/>
       <c r="I164" s="14"/>
       <c r="J164" s="14"/>
@@ -7692,7 +7685,7 @@
       <c r="D165" s="20"/>
       <c r="E165" s="14"/>
       <c r="F165" s="20"/>
-      <c r="G165" s="24"/>
+      <c r="G165" s="23"/>
       <c r="H165" s="14"/>
       <c r="I165" s="14"/>
       <c r="J165" s="14"/>
@@ -7726,7 +7719,7 @@
       <c r="D166" s="20"/>
       <c r="E166" s="14"/>
       <c r="F166" s="20"/>
-      <c r="G166" s="24"/>
+      <c r="G166" s="23"/>
       <c r="H166" s="14"/>
       <c r="I166" s="14"/>
       <c r="J166" s="14"/>
@@ -7760,7 +7753,7 @@
       <c r="D167" s="20"/>
       <c r="E167" s="14"/>
       <c r="F167" s="20"/>
-      <c r="G167" s="24"/>
+      <c r="G167" s="23"/>
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
       <c r="J167" s="14"/>
@@ -7794,7 +7787,7 @@
       <c r="D168" s="20"/>
       <c r="E168" s="14"/>
       <c r="F168" s="20"/>
-      <c r="G168" s="24"/>
+      <c r="G168" s="23"/>
       <c r="H168" s="14"/>
       <c r="I168" s="14"/>
       <c r="J168" s="14"/>
@@ -7828,7 +7821,7 @@
       <c r="D169" s="20"/>
       <c r="E169" s="14"/>
       <c r="F169" s="20"/>
-      <c r="G169" s="24"/>
+      <c r="G169" s="23"/>
       <c r="H169" s="14"/>
       <c r="I169" s="14"/>
       <c r="J169" s="14"/>
@@ -7862,7 +7855,7 @@
       <c r="D170" s="20"/>
       <c r="E170" s="14"/>
       <c r="F170" s="20"/>
-      <c r="G170" s="24"/>
+      <c r="G170" s="23"/>
       <c r="H170" s="14"/>
       <c r="I170" s="14"/>
       <c r="J170" s="14"/>
@@ -7896,7 +7889,7 @@
       <c r="D171" s="20"/>
       <c r="E171" s="14"/>
       <c r="F171" s="20"/>
-      <c r="G171" s="24"/>
+      <c r="G171" s="23"/>
       <c r="H171" s="14"/>
       <c r="I171" s="14"/>
       <c r="J171" s="14"/>
@@ -7930,7 +7923,7 @@
       <c r="D172" s="20"/>
       <c r="E172" s="14"/>
       <c r="F172" s="20"/>
-      <c r="G172" s="24"/>
+      <c r="G172" s="23"/>
       <c r="H172" s="14"/>
       <c r="I172" s="14"/>
       <c r="J172" s="14"/>
@@ -7964,7 +7957,7 @@
       <c r="D173" s="20"/>
       <c r="E173" s="14"/>
       <c r="F173" s="20"/>
-      <c r="G173" s="24"/>
+      <c r="G173" s="23"/>
       <c r="H173" s="14"/>
       <c r="I173" s="14"/>
       <c r="J173" s="14"/>
@@ -7998,7 +7991,7 @@
       <c r="D174" s="20"/>
       <c r="E174" s="14"/>
       <c r="F174" s="20"/>
-      <c r="G174" s="24"/>
+      <c r="G174" s="23"/>
       <c r="H174" s="14"/>
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
@@ -8032,7 +8025,7 @@
       <c r="D175" s="20"/>
       <c r="E175" s="14"/>
       <c r="F175" s="20"/>
-      <c r="G175" s="24"/>
+      <c r="G175" s="23"/>
       <c r="H175" s="14"/>
       <c r="I175" s="14"/>
       <c r="J175" s="14"/>
@@ -8066,7 +8059,7 @@
       <c r="D176" s="20"/>
       <c r="E176" s="14"/>
       <c r="F176" s="20"/>
-      <c r="G176" s="24"/>
+      <c r="G176" s="23"/>
       <c r="H176" s="14"/>
       <c r="I176" s="14"/>
       <c r="J176" s="14"/>
@@ -8100,7 +8093,7 @@
       <c r="D177" s="20"/>
       <c r="E177" s="14"/>
       <c r="F177" s="20"/>
-      <c r="G177" s="24"/>
+      <c r="G177" s="23"/>
       <c r="H177" s="14"/>
       <c r="I177" s="14"/>
       <c r="J177" s="14"/>
@@ -8134,7 +8127,7 @@
       <c r="D178" s="20"/>
       <c r="E178" s="14"/>
       <c r="F178" s="20"/>
-      <c r="G178" s="24"/>
+      <c r="G178" s="23"/>
       <c r="H178" s="14"/>
       <c r="I178" s="14"/>
       <c r="J178" s="14"/>
@@ -8168,7 +8161,7 @@
       <c r="D179" s="20"/>
       <c r="E179" s="14"/>
       <c r="F179" s="20"/>
-      <c r="G179" s="24"/>
+      <c r="G179" s="23"/>
       <c r="H179" s="14"/>
       <c r="I179" s="14"/>
       <c r="J179" s="14"/>
@@ -8202,7 +8195,7 @@
       <c r="D180" s="20"/>
       <c r="E180" s="14"/>
       <c r="F180" s="20"/>
-      <c r="G180" s="24"/>
+      <c r="G180" s="23"/>
       <c r="H180" s="14"/>
       <c r="I180" s="14"/>
       <c r="J180" s="14"/>
@@ -8236,7 +8229,7 @@
       <c r="D181" s="20"/>
       <c r="E181" s="14"/>
       <c r="F181" s="20"/>
-      <c r="G181" s="24"/>
+      <c r="G181" s="23"/>
       <c r="H181" s="14"/>
       <c r="I181" s="14"/>
       <c r="J181" s="14"/>
@@ -8270,7 +8263,7 @@
       <c r="D182" s="20"/>
       <c r="E182" s="14"/>
       <c r="F182" s="20"/>
-      <c r="G182" s="24"/>
+      <c r="G182" s="23"/>
       <c r="H182" s="14"/>
       <c r="I182" s="14"/>
       <c r="J182" s="14"/>
@@ -8304,7 +8297,7 @@
       <c r="D183" s="20"/>
       <c r="E183" s="14"/>
       <c r="F183" s="20"/>
-      <c r="G183" s="24"/>
+      <c r="G183" s="23"/>
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="14"/>
@@ -8338,7 +8331,7 @@
       <c r="D184" s="20"/>
       <c r="E184" s="14"/>
       <c r="F184" s="20"/>
-      <c r="G184" s="24"/>
+      <c r="G184" s="23"/>
       <c r="H184" s="14"/>
       <c r="I184" s="14"/>
       <c r="J184" s="14"/>
@@ -8372,7 +8365,7 @@
       <c r="D185" s="20"/>
       <c r="E185" s="14"/>
       <c r="F185" s="20"/>
-      <c r="G185" s="24"/>
+      <c r="G185" s="23"/>
       <c r="H185" s="14"/>
       <c r="I185" s="14"/>
       <c r="J185" s="14"/>
@@ -8406,7 +8399,7 @@
       <c r="D186" s="20"/>
       <c r="E186" s="14"/>
       <c r="F186" s="20"/>
-      <c r="G186" s="24"/>
+      <c r="G186" s="23"/>
       <c r="H186" s="14"/>
       <c r="I186" s="14"/>
       <c r="J186" s="14"/>
@@ -8440,7 +8433,7 @@
       <c r="D187" s="20"/>
       <c r="E187" s="14"/>
       <c r="F187" s="20"/>
-      <c r="G187" s="24"/>
+      <c r="G187" s="23"/>
       <c r="H187" s="14"/>
       <c r="I187" s="14"/>
       <c r="J187" s="14"/>
@@ -8474,7 +8467,7 @@
       <c r="D188" s="20"/>
       <c r="E188" s="14"/>
       <c r="F188" s="20"/>
-      <c r="G188" s="24"/>
+      <c r="G188" s="23"/>
       <c r="H188" s="14"/>
       <c r="I188" s="14"/>
       <c r="J188" s="14"/>
@@ -8508,7 +8501,7 @@
       <c r="D189" s="20"/>
       <c r="E189" s="14"/>
       <c r="F189" s="20"/>
-      <c r="G189" s="24"/>
+      <c r="G189" s="23"/>
       <c r="H189" s="14"/>
       <c r="I189" s="14"/>
       <c r="J189" s="14"/>
@@ -8542,7 +8535,7 @@
       <c r="D190" s="20"/>
       <c r="E190" s="14"/>
       <c r="F190" s="20"/>
-      <c r="G190" s="24"/>
+      <c r="G190" s="23"/>
       <c r="H190" s="14"/>
       <c r="I190" s="14"/>
       <c r="J190" s="14"/>
@@ -8576,7 +8569,7 @@
       <c r="D191" s="20"/>
       <c r="E191" s="14"/>
       <c r="F191" s="20"/>
-      <c r="G191" s="24"/>
+      <c r="G191" s="23"/>
       <c r="H191" s="14"/>
       <c r="I191" s="14"/>
       <c r="J191" s="14"/>
@@ -8610,7 +8603,7 @@
       <c r="D192" s="20"/>
       <c r="E192" s="14"/>
       <c r="F192" s="20"/>
-      <c r="G192" s="24"/>
+      <c r="G192" s="23"/>
       <c r="H192" s="14"/>
       <c r="I192" s="14"/>
       <c r="J192" s="14"/>
@@ -8644,7 +8637,7 @@
       <c r="D193" s="20"/>
       <c r="E193" s="14"/>
       <c r="F193" s="20"/>
-      <c r="G193" s="24"/>
+      <c r="G193" s="23"/>
       <c r="H193" s="14"/>
       <c r="I193" s="14"/>
       <c r="J193" s="14"/>
@@ -8678,7 +8671,7 @@
       <c r="D194" s="20"/>
       <c r="E194" s="14"/>
       <c r="F194" s="20"/>
-      <c r="G194" s="24"/>
+      <c r="G194" s="23"/>
       <c r="H194" s="14"/>
       <c r="I194" s="14"/>
       <c r="J194" s="14"/>
@@ -8712,7 +8705,7 @@
       <c r="D195" s="20"/>
       <c r="E195" s="14"/>
       <c r="F195" s="20"/>
-      <c r="G195" s="24"/>
+      <c r="G195" s="23"/>
       <c r="H195" s="14"/>
       <c r="I195" s="14"/>
       <c r="J195" s="14"/>
@@ -8746,7 +8739,7 @@
       <c r="D196" s="20"/>
       <c r="E196" s="14"/>
       <c r="F196" s="20"/>
-      <c r="G196" s="24"/>
+      <c r="G196" s="23"/>
       <c r="H196" s="14"/>
       <c r="I196" s="14"/>
       <c r="J196" s="14"/>
@@ -8780,7 +8773,7 @@
       <c r="D197" s="20"/>
       <c r="E197" s="14"/>
       <c r="F197" s="20"/>
-      <c r="G197" s="24"/>
+      <c r="G197" s="23"/>
       <c r="H197" s="14"/>
       <c r="I197" s="14"/>
       <c r="J197" s="14"/>
@@ -8814,7 +8807,7 @@
       <c r="D198" s="20"/>
       <c r="E198" s="14"/>
       <c r="F198" s="20"/>
-      <c r="G198" s="24"/>
+      <c r="G198" s="23"/>
       <c r="H198" s="14"/>
       <c r="I198" s="14"/>
       <c r="J198" s="14"/>
@@ -8848,7 +8841,7 @@
       <c r="D199" s="20"/>
       <c r="E199" s="14"/>
       <c r="F199" s="20"/>
-      <c r="G199" s="24"/>
+      <c r="G199" s="23"/>
       <c r="H199" s="14"/>
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
@@ -8882,7 +8875,7 @@
       <c r="D200" s="20"/>
       <c r="E200" s="14"/>
       <c r="F200" s="20"/>
-      <c r="G200" s="24"/>
+      <c r="G200" s="23"/>
       <c r="H200" s="14"/>
       <c r="I200" s="14"/>
       <c r="J200" s="14"/>
@@ -8916,7 +8909,7 @@
       <c r="D201" s="20"/>
       <c r="E201" s="14"/>
       <c r="F201" s="20"/>
-      <c r="G201" s="24"/>
+      <c r="G201" s="23"/>
       <c r="H201" s="14"/>
       <c r="I201" s="14"/>
       <c r="J201" s="14"/>
@@ -8950,7 +8943,7 @@
       <c r="D202" s="20"/>
       <c r="E202" s="14"/>
       <c r="F202" s="20"/>
-      <c r="G202" s="24"/>
+      <c r="G202" s="23"/>
       <c r="H202" s="14"/>
       <c r="I202" s="14"/>
       <c r="J202" s="14"/>
@@ -8984,7 +8977,7 @@
       <c r="D203" s="20"/>
       <c r="E203" s="14"/>
       <c r="F203" s="20"/>
-      <c r="G203" s="24"/>
+      <c r="G203" s="23"/>
       <c r="H203" s="14"/>
       <c r="I203" s="14"/>
       <c r="J203" s="14"/>
@@ -9018,7 +9011,7 @@
       <c r="D204" s="20"/>
       <c r="E204" s="14"/>
       <c r="F204" s="20"/>
-      <c r="G204" s="24"/>
+      <c r="G204" s="23"/>
       <c r="H204" s="14"/>
       <c r="I204" s="14"/>
       <c r="J204" s="14"/>
@@ -9052,7 +9045,7 @@
       <c r="D205" s="20"/>
       <c r="E205" s="14"/>
       <c r="F205" s="20"/>
-      <c r="G205" s="24"/>
+      <c r="G205" s="23"/>
       <c r="H205" s="14"/>
       <c r="I205" s="14"/>
       <c r="J205" s="14"/>
@@ -9086,7 +9079,7 @@
       <c r="D206" s="20"/>
       <c r="E206" s="14"/>
       <c r="F206" s="20"/>
-      <c r="G206" s="24"/>
+      <c r="G206" s="23"/>
       <c r="H206" s="14"/>
       <c r="I206" s="14"/>
       <c r="J206" s="14"/>
@@ -9120,7 +9113,7 @@
       <c r="D207" s="20"/>
       <c r="E207" s="14"/>
       <c r="F207" s="20"/>
-      <c r="G207" s="24"/>
+      <c r="G207" s="23"/>
       <c r="H207" s="14"/>
       <c r="I207" s="14"/>
       <c r="J207" s="14"/>
@@ -9154,7 +9147,7 @@
       <c r="D208" s="20"/>
       <c r="E208" s="14"/>
       <c r="F208" s="20"/>
-      <c r="G208" s="24"/>
+      <c r="G208" s="23"/>
       <c r="H208" s="14"/>
       <c r="I208" s="14"/>
       <c r="J208" s="14"/>
@@ -9188,7 +9181,7 @@
       <c r="D209" s="20"/>
       <c r="E209" s="14"/>
       <c r="F209" s="20"/>
-      <c r="G209" s="24"/>
+      <c r="G209" s="23"/>
       <c r="H209" s="14"/>
       <c r="I209" s="14"/>
       <c r="J209" s="14"/>
@@ -9222,7 +9215,7 @@
       <c r="D210" s="20"/>
       <c r="E210" s="14"/>
       <c r="F210" s="20"/>
-      <c r="G210" s="24"/>
+      <c r="G210" s="23"/>
       <c r="H210" s="14"/>
       <c r="I210" s="14"/>
       <c r="J210" s="14"/>
@@ -9256,7 +9249,7 @@
       <c r="D211" s="20"/>
       <c r="E211" s="14"/>
       <c r="F211" s="20"/>
-      <c r="G211" s="24"/>
+      <c r="G211" s="23"/>
       <c r="H211" s="14"/>
       <c r="I211" s="14"/>
       <c r="J211" s="14"/>
@@ -9290,7 +9283,7 @@
       <c r="D212" s="20"/>
       <c r="E212" s="14"/>
       <c r="F212" s="20"/>
-      <c r="G212" s="24"/>
+      <c r="G212" s="23"/>
       <c r="H212" s="14"/>
       <c r="I212" s="14"/>
       <c r="J212" s="14"/>
@@ -9324,7 +9317,7 @@
       <c r="D213" s="20"/>
       <c r="E213" s="14"/>
       <c r="F213" s="20"/>
-      <c r="G213" s="24"/>
+      <c r="G213" s="23"/>
       <c r="H213" s="14"/>
       <c r="I213" s="14"/>
       <c r="J213" s="14"/>
@@ -9358,7 +9351,7 @@
       <c r="D214" s="20"/>
       <c r="E214" s="14"/>
       <c r="F214" s="20"/>
-      <c r="G214" s="24"/>
+      <c r="G214" s="23"/>
       <c r="H214" s="14"/>
       <c r="I214" s="14"/>
       <c r="J214" s="14"/>
@@ -9392,7 +9385,7 @@
       <c r="D215" s="20"/>
       <c r="E215" s="14"/>
       <c r="F215" s="20"/>
-      <c r="G215" s="24"/>
+      <c r="G215" s="23"/>
       <c r="H215" s="14"/>
       <c r="I215" s="14"/>
       <c r="J215" s="14"/>
@@ -9426,7 +9419,7 @@
       <c r="D216" s="20"/>
       <c r="E216" s="14"/>
       <c r="F216" s="20"/>
-      <c r="G216" s="24"/>
+      <c r="G216" s="23"/>
       <c r="H216" s="14"/>
       <c r="I216" s="14"/>
       <c r="J216" s="14"/>
@@ -9460,7 +9453,7 @@
       <c r="D217" s="20"/>
       <c r="E217" s="14"/>
       <c r="F217" s="20"/>
-      <c r="G217" s="24"/>
+      <c r="G217" s="23"/>
       <c r="H217" s="14"/>
       <c r="I217" s="14"/>
       <c r="J217" s="14"/>
@@ -9494,7 +9487,7 @@
       <c r="D218" s="20"/>
       <c r="E218" s="14"/>
       <c r="F218" s="20"/>
-      <c r="G218" s="24"/>
+      <c r="G218" s="23"/>
       <c r="H218" s="14"/>
       <c r="I218" s="14"/>
       <c r="J218" s="14"/>
@@ -9528,7 +9521,7 @@
       <c r="D219" s="20"/>
       <c r="E219" s="14"/>
       <c r="F219" s="20"/>
-      <c r="G219" s="24"/>
+      <c r="G219" s="23"/>
       <c r="H219" s="14"/>
       <c r="I219" s="14"/>
       <c r="J219" s="14"/>
@@ -9562,7 +9555,7 @@
       <c r="D220" s="20"/>
       <c r="E220" s="14"/>
       <c r="F220" s="20"/>
-      <c r="G220" s="24"/>
+      <c r="G220" s="23"/>
       <c r="H220" s="14"/>
       <c r="I220" s="14"/>
       <c r="J220" s="14"/>
@@ -9596,7 +9589,7 @@
       <c r="D221" s="20"/>
       <c r="E221" s="14"/>
       <c r="F221" s="20"/>
-      <c r="G221" s="24"/>
+      <c r="G221" s="23"/>
       <c r="H221" s="14"/>
       <c r="I221" s="14"/>
       <c r="J221" s="14"/>
@@ -9630,7 +9623,7 @@
       <c r="D222" s="20"/>
       <c r="E222" s="14"/>
       <c r="F222" s="20"/>
-      <c r="G222" s="24"/>
+      <c r="G222" s="23"/>
       <c r="H222" s="14"/>
       <c r="I222" s="14"/>
       <c r="J222" s="14"/>
@@ -9664,7 +9657,7 @@
       <c r="D223" s="20"/>
       <c r="E223" s="14"/>
       <c r="F223" s="20"/>
-      <c r="G223" s="24"/>
+      <c r="G223" s="23"/>
       <c r="H223" s="14"/>
       <c r="I223" s="14"/>
       <c r="J223" s="14"/>
@@ -9698,7 +9691,7 @@
       <c r="D224" s="20"/>
       <c r="E224" s="14"/>
       <c r="F224" s="20"/>
-      <c r="G224" s="24"/>
+      <c r="G224" s="23"/>
       <c r="H224" s="14"/>
       <c r="I224" s="14"/>
       <c r="J224" s="14"/>
@@ -9732,7 +9725,7 @@
       <c r="D225" s="20"/>
       <c r="E225" s="14"/>
       <c r="F225" s="20"/>
-      <c r="G225" s="24"/>
+      <c r="G225" s="23"/>
       <c r="H225" s="14"/>
       <c r="I225" s="14"/>
       <c r="J225" s="14"/>
@@ -9766,7 +9759,7 @@
       <c r="D226" s="20"/>
       <c r="E226" s="14"/>
       <c r="F226" s="20"/>
-      <c r="G226" s="24"/>
+      <c r="G226" s="23"/>
       <c r="H226" s="14"/>
       <c r="I226" s="14"/>
       <c r="J226" s="14"/>
@@ -9800,7 +9793,7 @@
       <c r="D227" s="20"/>
       <c r="E227" s="14"/>
       <c r="F227" s="20"/>
-      <c r="G227" s="24"/>
+      <c r="G227" s="23"/>
       <c r="H227" s="14"/>
       <c r="I227" s="14"/>
       <c r="J227" s="14"/>
@@ -9834,7 +9827,7 @@
       <c r="D228" s="20"/>
       <c r="E228" s="14"/>
       <c r="F228" s="20"/>
-      <c r="G228" s="24"/>
+      <c r="G228" s="23"/>
       <c r="H228" s="14"/>
       <c r="I228" s="14"/>
       <c r="J228" s="14"/>
@@ -9868,7 +9861,7 @@
       <c r="D229" s="20"/>
       <c r="E229" s="14"/>
       <c r="F229" s="20"/>
-      <c r="G229" s="24"/>
+      <c r="G229" s="23"/>
       <c r="H229" s="14"/>
       <c r="I229" s="14"/>
       <c r="J229" s="14"/>
@@ -9902,7 +9895,7 @@
       <c r="D230" s="20"/>
       <c r="E230" s="14"/>
       <c r="F230" s="20"/>
-      <c r="G230" s="24"/>
+      <c r="G230" s="23"/>
       <c r="H230" s="14"/>
       <c r="I230" s="14"/>
       <c r="J230" s="14"/>
@@ -9936,7 +9929,7 @@
       <c r="D231" s="20"/>
       <c r="E231" s="14"/>
       <c r="F231" s="20"/>
-      <c r="G231" s="24"/>
+      <c r="G231" s="23"/>
       <c r="H231" s="14"/>
       <c r="I231" s="14"/>
       <c r="J231" s="14"/>
@@ -9970,7 +9963,7 @@
       <c r="D232" s="20"/>
       <c r="E232" s="14"/>
       <c r="F232" s="20"/>
-      <c r="G232" s="24"/>
+      <c r="G232" s="23"/>
       <c r="H232" s="14"/>
       <c r="I232" s="14"/>
       <c r="J232" s="14"/>
@@ -10004,7 +9997,7 @@
       <c r="D233" s="20"/>
       <c r="E233" s="14"/>
       <c r="F233" s="20"/>
-      <c r="G233" s="24"/>
+      <c r="G233" s="23"/>
       <c r="H233" s="14"/>
       <c r="I233" s="14"/>
       <c r="J233" s="14"/>
@@ -10038,7 +10031,7 @@
       <c r="D234" s="20"/>
       <c r="E234" s="14"/>
       <c r="F234" s="20"/>
-      <c r="G234" s="24"/>
+      <c r="G234" s="23"/>
       <c r="H234" s="14"/>
       <c r="I234" s="14"/>
       <c r="J234" s="14"/>
@@ -10072,7 +10065,7 @@
       <c r="D235" s="20"/>
       <c r="E235" s="14"/>
       <c r="F235" s="20"/>
-      <c r="G235" s="24"/>
+      <c r="G235" s="23"/>
       <c r="H235" s="14"/>
       <c r="I235" s="14"/>
       <c r="J235" s="14"/>
@@ -10106,7 +10099,7 @@
       <c r="D236" s="20"/>
       <c r="E236" s="14"/>
       <c r="F236" s="20"/>
-      <c r="G236" s="24"/>
+      <c r="G236" s="23"/>
       <c r="H236" s="14"/>
       <c r="I236" s="14"/>
       <c r="J236" s="14"/>
@@ -10140,7 +10133,7 @@
       <c r="D237" s="20"/>
       <c r="E237" s="14"/>
       <c r="F237" s="20"/>
-      <c r="G237" s="24"/>
+      <c r="G237" s="23"/>
       <c r="H237" s="14"/>
       <c r="I237" s="14"/>
       <c r="J237" s="14"/>
@@ -10174,7 +10167,7 @@
       <c r="D238" s="20"/>
       <c r="E238" s="14"/>
       <c r="F238" s="20"/>
-      <c r="G238" s="24"/>
+      <c r="G238" s="23"/>
       <c r="H238" s="14"/>
       <c r="I238" s="14"/>
       <c r="J238" s="14"/>
@@ -10208,7 +10201,7 @@
       <c r="D239" s="20"/>
       <c r="E239" s="14"/>
       <c r="F239" s="20"/>
-      <c r="G239" s="24"/>
+      <c r="G239" s="23"/>
       <c r="H239" s="14"/>
       <c r="I239" s="14"/>
       <c r="J239" s="14"/>
@@ -10242,7 +10235,7 @@
       <c r="D240" s="20"/>
       <c r="E240" s="14"/>
       <c r="F240" s="20"/>
-      <c r="G240" s="24"/>
+      <c r="G240" s="23"/>
       <c r="H240" s="14"/>
       <c r="I240" s="14"/>
       <c r="J240" s="14"/>
@@ -10276,7 +10269,7 @@
       <c r="D241" s="20"/>
       <c r="E241" s="14"/>
       <c r="F241" s="20"/>
-      <c r="G241" s="24"/>
+      <c r="G241" s="23"/>
       <c r="H241" s="14"/>
       <c r="I241" s="14"/>
       <c r="J241" s="14"/>
@@ -10310,7 +10303,7 @@
       <c r="D242" s="20"/>
       <c r="E242" s="14"/>
       <c r="F242" s="20"/>
-      <c r="G242" s="24"/>
+      <c r="G242" s="23"/>
       <c r="H242" s="14"/>
       <c r="I242" s="14"/>
       <c r="J242" s="14"/>
@@ -10344,7 +10337,7 @@
       <c r="D243" s="20"/>
       <c r="E243" s="14"/>
       <c r="F243" s="20"/>
-      <c r="G243" s="24"/>
+      <c r="G243" s="23"/>
       <c r="H243" s="14"/>
       <c r="I243" s="14"/>
       <c r="J243" s="14"/>
@@ -10378,7 +10371,7 @@
       <c r="D244" s="20"/>
       <c r="E244" s="14"/>
       <c r="F244" s="20"/>
-      <c r="G244" s="24"/>
+      <c r="G244" s="23"/>
       <c r="H244" s="14"/>
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
@@ -10412,7 +10405,7 @@
       <c r="D245" s="20"/>
       <c r="E245" s="14"/>
       <c r="F245" s="20"/>
-      <c r="G245" s="24"/>
+      <c r="G245" s="23"/>
       <c r="H245" s="14"/>
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
@@ -10446,7 +10439,7 @@
       <c r="D246" s="20"/>
       <c r="E246" s="14"/>
       <c r="F246" s="20"/>
-      <c r="G246" s="24"/>
+      <c r="G246" s="23"/>
       <c r="H246" s="14"/>
       <c r="I246" s="14"/>
       <c r="J246" s="14"/>
@@ -10480,7 +10473,7 @@
       <c r="D247" s="20"/>
       <c r="E247" s="14"/>
       <c r="F247" s="20"/>
-      <c r="G247" s="24"/>
+      <c r="G247" s="23"/>
       <c r="H247" s="14"/>
       <c r="I247" s="14"/>
       <c r="J247" s="14"/>
@@ -10514,7 +10507,7 @@
       <c r="D248" s="20"/>
       <c r="E248" s="14"/>
       <c r="F248" s="20"/>
-      <c r="G248" s="24"/>
+      <c r="G248" s="23"/>
       <c r="H248" s="14"/>
       <c r="I248" s="14"/>
       <c r="J248" s="14"/>
@@ -10548,7 +10541,7 @@
       <c r="D249" s="20"/>
       <c r="E249" s="14"/>
       <c r="F249" s="20"/>
-      <c r="G249" s="24"/>
+      <c r="G249" s="23"/>
       <c r="H249" s="14"/>
       <c r="I249" s="14"/>
       <c r="J249" s="14"/>
@@ -10582,7 +10575,7 @@
       <c r="D250" s="20"/>
       <c r="E250" s="14"/>
       <c r="F250" s="20"/>
-      <c r="G250" s="24"/>
+      <c r="G250" s="23"/>
       <c r="H250" s="14"/>
       <c r="I250" s="14"/>
       <c r="J250" s="14"/>
@@ -10616,7 +10609,7 @@
       <c r="D251" s="20"/>
       <c r="E251" s="14"/>
       <c r="F251" s="20"/>
-      <c r="G251" s="24"/>
+      <c r="G251" s="23"/>
       <c r="H251" s="14"/>
       <c r="I251" s="14"/>
       <c r="J251" s="14"/>
@@ -10650,7 +10643,7 @@
       <c r="D252" s="20"/>
       <c r="E252" s="14"/>
       <c r="F252" s="20"/>
-      <c r="G252" s="24"/>
+      <c r="G252" s="23"/>
       <c r="H252" s="14"/>
       <c r="I252" s="14"/>
       <c r="J252" s="14"/>
@@ -10684,7 +10677,7 @@
       <c r="D253" s="20"/>
       <c r="E253" s="14"/>
       <c r="F253" s="20"/>
-      <c r="G253" s="24"/>
+      <c r="G253" s="23"/>
       <c r="H253" s="14"/>
       <c r="I253" s="14"/>
       <c r="J253" s="14"/>
@@ -10718,7 +10711,7 @@
       <c r="D254" s="20"/>
       <c r="E254" s="14"/>
       <c r="F254" s="20"/>
-      <c r="G254" s="24"/>
+      <c r="G254" s="23"/>
       <c r="H254" s="14"/>
       <c r="I254" s="14"/>
       <c r="J254" s="14"/>
@@ -10752,7 +10745,7 @@
       <c r="D255" s="20"/>
       <c r="E255" s="14"/>
       <c r="F255" s="20"/>
-      <c r="G255" s="24"/>
+      <c r="G255" s="23"/>
       <c r="H255" s="14"/>
       <c r="I255" s="14"/>
       <c r="J255" s="14"/>
@@ -10786,7 +10779,7 @@
       <c r="D256" s="20"/>
       <c r="E256" s="14"/>
       <c r="F256" s="20"/>
-      <c r="G256" s="24"/>
+      <c r="G256" s="23"/>
       <c r="H256" s="14"/>
       <c r="I256" s="14"/>
       <c r="J256" s="14"/>
@@ -10820,7 +10813,7 @@
       <c r="D257" s="20"/>
       <c r="E257" s="14"/>
       <c r="F257" s="20"/>
-      <c r="G257" s="24"/>
+      <c r="G257" s="23"/>
       <c r="H257" s="14"/>
       <c r="I257" s="14"/>
       <c r="J257" s="14"/>
@@ -10854,7 +10847,7 @@
       <c r="D258" s="20"/>
       <c r="E258" s="14"/>
       <c r="F258" s="20"/>
-      <c r="G258" s="24"/>
+      <c r="G258" s="23"/>
       <c r="H258" s="14"/>
       <c r="I258" s="14"/>
       <c r="J258" s="14"/>
@@ -10888,7 +10881,7 @@
       <c r="D259" s="20"/>
       <c r="E259" s="14"/>
       <c r="F259" s="20"/>
-      <c r="G259" s="24"/>
+      <c r="G259" s="23"/>
       <c r="H259" s="14"/>
       <c r="I259" s="14"/>
       <c r="J259" s="14"/>
@@ -10922,7 +10915,7 @@
       <c r="D260" s="20"/>
       <c r="E260" s="14"/>
       <c r="F260" s="20"/>
-      <c r="G260" s="24"/>
+      <c r="G260" s="23"/>
       <c r="H260" s="14"/>
       <c r="I260" s="14"/>
       <c r="J260" s="14"/>
@@ -10956,7 +10949,7 @@
       <c r="D261" s="20"/>
       <c r="E261" s="14"/>
       <c r="F261" s="20"/>
-      <c r="G261" s="24"/>
+      <c r="G261" s="23"/>
       <c r="H261" s="14"/>
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
@@ -10990,7 +10983,7 @@
       <c r="D262" s="20"/>
       <c r="E262" s="14"/>
       <c r="F262" s="20"/>
-      <c r="G262" s="24"/>
+      <c r="G262" s="23"/>
       <c r="H262" s="14"/>
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
@@ -11024,7 +11017,7 @@
       <c r="D263" s="20"/>
       <c r="E263" s="14"/>
       <c r="F263" s="20"/>
-      <c r="G263" s="24"/>
+      <c r="G263" s="23"/>
       <c r="H263" s="14"/>
       <c r="I263" s="14"/>
       <c r="J263" s="14"/>
@@ -11058,7 +11051,7 @@
       <c r="D264" s="20"/>
       <c r="E264" s="14"/>
       <c r="F264" s="20"/>
-      <c r="G264" s="24"/>
+      <c r="G264" s="23"/>
       <c r="H264" s="14"/>
       <c r="I264" s="14"/>
       <c r="J264" s="14"/>
@@ -11092,7 +11085,7 @@
       <c r="D265" s="20"/>
       <c r="E265" s="14"/>
       <c r="F265" s="20"/>
-      <c r="G265" s="24"/>
+      <c r="G265" s="23"/>
       <c r="H265" s="14"/>
       <c r="I265" s="14"/>
       <c r="J265" s="14"/>
@@ -11126,7 +11119,7 @@
       <c r="D266" s="20"/>
       <c r="E266" s="14"/>
       <c r="F266" s="20"/>
-      <c r="G266" s="24"/>
+      <c r="G266" s="23"/>
       <c r="H266" s="14"/>
       <c r="I266" s="14"/>
       <c r="J266" s="14"/>
@@ -11160,7 +11153,7 @@
       <c r="D267" s="20"/>
       <c r="E267" s="14"/>
       <c r="F267" s="20"/>
-      <c r="G267" s="24"/>
+      <c r="G267" s="23"/>
       <c r="H267" s="14"/>
       <c r="I267" s="14"/>
       <c r="J267" s="14"/>
@@ -11195,12 +11188,16 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Si RADIE: indiquez ici la date de radiation" sqref="L2:L1048576" xr:uid="{9C6DAB79-C794-3A44-ABF5-3A0809655B2F}"/>
     <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Format : jj/mm/aaa_x000a_Ex: 20/12/1991" sqref="E2:E1048576" xr:uid="{63D08891-D065-7B47-846B-3FB13801D5E9}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{1DB8D27B-8C74-DA4C-BEE9-5B682BEBC191}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{32163EC9-9906-1E43-8ABC-EE3E5692639D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="H2" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -11274,90 +11271,90 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11365,16 +11362,16 @@
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11384,10 +11381,10 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11397,10 +11394,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11409,7 +11406,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(usagers): correction d'un bug quand il n'y a aucun domicilié feat(usagers): possibilité de faire un hard reset des usagers fix(import): correction d'un bug sur le motif de refus "autre"
</commit_message>
<xml_diff>
--- a/packages/frontend/src/assets/files/modele.xlsx
+++ b/packages/frontend/src/assets/files/modele.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Google Drive/DomiFa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/frontend/src/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F9685-160D-8942-98E5-3984A0EFFD67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F6568-9E9F-6046-BEAE-77ABE10BDB83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{78346249-D4CA-EC45-AC14-C98ADBF7EA96}"/>
   </bookViews>
   <sheets>
     <sheet name="DOMICILIES" sheetId="2" r:id="rId1"/>
-    <sheet name="LISTE DÉROULANTES" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="LISTE DÉROULANTES" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>PREMIERE</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>HORS_AGREMENT</t>
-  </si>
-  <si>
-    <t>AUTRES</t>
   </si>
   <si>
     <t>HOMME_ISOLE_SANS_ENFANT</t>
@@ -1883,10 +1880,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667784FF-BEC0-7A46-B044-88051932373E}">
   <dimension ref="A1:AF267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1912,100 +1909,100 @@
   <sheetData>
     <row r="1" spans="1:32" s="13" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="P1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AC1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="15" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,23 +2010,23 @@
         <v>5</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>2</v>
@@ -2041,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>8</v>
@@ -2049,28 +2046,28 @@
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="20" t="s">
-        <v>95</v>
-      </c>
       <c r="S2" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W2" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X2" s="20" t="s">
         <v>14</v>
@@ -2089,20 +2086,20 @@
         <v>4</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>7</v>
@@ -2114,27 +2111,27 @@
         <v>1</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
       <c r="P3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="S3" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="T3" s="20" t="s">
         <v>16</v>
@@ -2157,19 +2154,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>69</v>
-      </c>
       <c r="E4" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="14"/>
@@ -2180,10 +2177,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4" s="14"/>
       <c r="N4" s="14" t="s">
@@ -2191,7 +2188,7 @@
       </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
@@ -2215,23 +2212,23 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -2243,17 +2240,17 @@
         <v>9</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M5" s="14" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
@@ -11255,7 +11252,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11286,10 +11283,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11309,10 +11306,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11332,10 +11329,10 @@
         <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11351,10 +11348,10 @@
         <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11365,13 +11362,13 @@
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11381,10 +11378,10 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11394,10 +11391,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -11406,7 +11403,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix(import): correction des données de l'entretien
</commit_message>
<xml_diff>
--- a/packages/frontend/src/assets/files/modele.xlsx
+++ b/packages/frontend/src/assets/files/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/frontend/src/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A7CD2F-143B-8D4B-9ABF-BF37403FFD7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488B7E7A-2E00-BE44-ADE5-54380D8599C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOMICILIES" sheetId="1" r:id="rId1"/>
@@ -593,61 +593,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12.5"/>
-        <color rgb="FF262626"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Si AUTRE motif, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12.5"/>
-        <color rgb="FF262626"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12.5"/>
-        <color rgb="FF262626"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>précisions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Seulement si accompagnement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12.5"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Par quelle structure est fait l'accompagnement?</t>
-    </r>
-  </si>
-  <si>
     <t>Quel est le lien avec la commune ? 
 (Si CCAS ou CIAS)</t>
   </si>
@@ -711,6 +656,61 @@
         <family val="2"/>
       </rPr>
       <t>(colonne à remplir uniquement en cas d'ID personnalisés)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Seulement si accompagnement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.5"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Par quelle structure est fait l'accompagnement?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12.5"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Si AUTRE motif,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12.5"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.5"/>
+        <color rgb="FF262626"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>précisions</t>
     </r>
   </si>
 </sst>
@@ -1133,18 +1133,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="57">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2520,30 +2508,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12.5"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2578,10 +2542,46 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12.5"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2633,57 +2633,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AW999" headerRowDxfId="50" dataDxfId="0" totalsRowDxfId="51" headerRowBorderDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AW999" headerRowDxfId="53" dataDxfId="51" totalsRowDxfId="49" headerRowBorderDxfId="52" tableBorderDxfId="50">
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID _x000a_(colonne à remplir uniquement en cas d'ID personnalisés)" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Civilité" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Nom de naissance" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Prénom" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nom d'usage / Surnom" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date de naissance" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Lieu de naissance" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Numéro de téléphone" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Adresse e-mail" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Statut de la domiciliation" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Seulement si refus_x000a_Motif du refus" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Seulement si radié_x000a_Motif de radiation" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Type de domiciliation" dataDxfId="37"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Date début dom actuelle" dataDxfId="36"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Date de fin de domiciliation_x000a_OU_x000a_Date de radiation si radié_x000a_OU _x000a_Date de refus si refusé" dataDxfId="35"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Date 1ere domiciliation" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{F3EC0B77-5925-4549-B090-3175E9AD69D3}" name="Date de dernier passage _x000a_(si vide, la date sera celle de l'import)" dataDxfId="33"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="La personne a-t-elle été orientée ?" dataDxfId="32"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Seulement si orientation _x000a_Par quelle structure/personne la personne a-t-elle été orientée ?" dataDxfId="31"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="La personne a-t-elle déjà une domiciliation ?" dataDxfId="30"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="La personne a-t-elle des revenus ?" dataDxfId="29"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Seulement si revenus_x000a_De quelle nature ?" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Quel est le lien avec la commune ? _x000a_(Si CCAS ou CIAS)" dataDxfId="27"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Composition du ménage" dataDxfId="26"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Situation résidentielle" dataDxfId="25"/>
-    <tableColumn id="45" xr3:uid="{973BA99D-2099-8447-A5F6-C95462E9533B}" name="Si AUTRE situation résidentielle_x000a_précisions" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cause de l'instabilité_x000a_ du logement" dataDxfId="23"/>
-    <tableColumn id="46" xr3:uid="{CAFD5E43-FC29-714C-BEA8-B5320362468C}" name="Si AUTRE cause d'instabilité_x000a_précisions" dataDxfId="22"/>
-    <tableColumn id="48" xr3:uid="{8A6DC35C-929D-2341-AFBA-85F886983314}" name="Quel est le motif principal de demande de domiciliation ?" dataDxfId="21"/>
-    <tableColumn id="47" xr3:uid="{A55284FD-ADFF-1848-88BD-250C0B85E5E4}" name="Si AUTRE motif, _x000a_précisions" dataDxfId="20"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Accompagnement social" dataDxfId="19"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Seulement si accompagnement _x000a_Par quelle structure est fait l'accompagnement?" dataDxfId="18"/>
-    <tableColumn id="49" xr3:uid="{2432BDAC-54A8-974C-BD03-3795C92EFD8C}" name="Commentaires _x000a_(1000 caractères maximum)" dataDxfId="17"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Nom Ayant-Droit 1" dataDxfId="16"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Prénom Ayant-Droit 1" dataDxfId="15"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Date de Naissance Ayant-Droit 1" dataDxfId="14"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Lien de parenté Ayant-Droit 1" dataDxfId="13"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Nom Ayant-Droit 2" dataDxfId="12"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Prénom Ayant-Droit 2" dataDxfId="11"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Date de Naissance Ayant-Droit 2" dataDxfId="10"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Lien de parenté Ayant-Droit 2" dataDxfId="9"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Nom Ayant-Droit 3" dataDxfId="8"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Prénom Ayant-Droit 3" dataDxfId="7"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Date de Naissance_x000a_Ayant-Droit 3" dataDxfId="6"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Lien de parenté_x000a_Ayant-Droit 3" dataDxfId="5"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Nom Ayant-Droit 4" dataDxfId="4"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Prénom Ayant-Droit 4" dataDxfId="3"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Date de Naissance Ayant-Droit 4" dataDxfId="2"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Lien de parenté Ayant-Droit 4" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID _x000a_(colonne à remplir uniquement en cas d'ID personnalisés)" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Civilité" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Nom de naissance" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Prénom" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nom d'usage / Surnom" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date de naissance" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Lieu de naissance" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Numéro de téléphone" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Adresse e-mail" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Statut de la domiciliation" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Seulement si refus_x000a_Motif du refus" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Seulement si radié_x000a_Motif de radiation" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Type de domiciliation" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Date début dom actuelle" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Date de fin de domiciliation_x000a_OU_x000a_Date de radiation si radié_x000a_OU _x000a_Date de refus si refusé" dataDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Date 1ere domiciliation" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{F3EC0B77-5925-4549-B090-3175E9AD69D3}" name="Date de dernier passage _x000a_(si vide, la date sera celle de l'import)" dataDxfId="32"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="La personne a-t-elle été orientée ?" dataDxfId="31"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Seulement si orientation _x000a_Par quelle structure/personne la personne a-t-elle été orientée ?" dataDxfId="30"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="La personne a-t-elle déjà une domiciliation ?" dataDxfId="29"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="La personne a-t-elle des revenus ?" dataDxfId="28"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Seulement si revenus_x000a_De quelle nature ?" dataDxfId="27"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Quel est le lien avec la commune ? _x000a_(Si CCAS ou CIAS)" dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Composition du ménage" dataDxfId="25"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Situation résidentielle" dataDxfId="24"/>
+    <tableColumn id="45" xr3:uid="{973BA99D-2099-8447-A5F6-C95462E9533B}" name="Si AUTRE situation résidentielle_x000a_précisions" dataDxfId="23"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cause de l'instabilité_x000a_ du logement" dataDxfId="22"/>
+    <tableColumn id="46" xr3:uid="{CAFD5E43-FC29-714C-BEA8-B5320362468C}" name="Si AUTRE cause d'instabilité_x000a_précisions" dataDxfId="21"/>
+    <tableColumn id="48" xr3:uid="{8A6DC35C-929D-2341-AFBA-85F886983314}" name="Quel est le motif principal de demande de domiciliation ?" dataDxfId="20"/>
+    <tableColumn id="47" xr3:uid="{A55284FD-ADFF-1848-88BD-250C0B85E5E4}" name="Si AUTRE motif,_x000a_précisions" dataDxfId="19"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Accompagnement social" dataDxfId="18"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Seulement si accompagnement_x000a_Par quelle structure est fait l'accompagnement?" dataDxfId="17"/>
+    <tableColumn id="49" xr3:uid="{2432BDAC-54A8-974C-BD03-3795C92EFD8C}" name="Commentaires _x000a_(1000 caractères maximum)" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Nom Ayant-Droit 1" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Prénom Ayant-Droit 1" dataDxfId="14"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Date de Naissance Ayant-Droit 1" dataDxfId="13"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Lien de parenté Ayant-Droit 1" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Nom Ayant-Droit 2" dataDxfId="11"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Prénom Ayant-Droit 2" dataDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Date de Naissance Ayant-Droit 2" dataDxfId="9"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Lien de parenté Ayant-Droit 2" dataDxfId="8"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Nom Ayant-Droit 3" dataDxfId="7"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Prénom Ayant-Droit 3" dataDxfId="6"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Date de Naissance_x000a_Ayant-Droit 3" dataDxfId="5"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Lien de parenté_x000a_Ayant-Droit 3" dataDxfId="4"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Nom Ayant-Droit 4" dataDxfId="3"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Prénom Ayant-Droit 4" dataDxfId="2"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Date de Naissance Ayant-Droit 4" dataDxfId="1"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Lien de parenté Ayant-Droit 4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="DOMICILIES-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2889,9 +2889,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S983" sqref="S983"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2923,14 +2923,15 @@
     <col min="27" max="27" width="33.28515625" style="13" customWidth="1"/>
     <col min="28" max="30" width="33.28515625" customWidth="1"/>
     <col min="31" max="31" width="29.28515625" style="13" customWidth="1"/>
-    <col min="32" max="33" width="29.42578125" customWidth="1"/>
+    <col min="32" max="32" width="32" customWidth="1"/>
+    <col min="33" max="33" width="29.42578125" customWidth="1"/>
     <col min="34" max="34" width="30.140625" customWidth="1"/>
     <col min="35" max="50" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="19" customFormat="1" ht="116" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -2960,10 +2961,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>9</v>
@@ -2987,7 +2988,7 @@
         <v>136</v>
       </c>
       <c r="T1" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="U1" s="16" t="s">
         <v>135</v>
@@ -2996,7 +2997,7 @@
         <v>137</v>
       </c>
       <c r="W1" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="X1" s="16" t="s">
         <v>12</v>
@@ -3017,13 +3018,13 @@
         <v>111</v>
       </c>
       <c r="AD1" s="16" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="AE1" s="16" t="s">
         <v>14</v>
       </c>
       <c r="AF1" s="17" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="AG1" s="17" t="s">
         <v>132</v>
@@ -54232,8 +54233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>